<commit_message>
Work in progress. Needs new compiler
</commit_message>
<xml_diff>
--- a/Runtime/RuntimeFunctionsAndClasses.xlsx
+++ b/Runtime/RuntimeFunctionsAndClasses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XSharp\DevRt\Runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{371029C1-D405-469D-998E-F0161E514FED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A9A41907-4EEA-4B5D-A5B5-84E9331AC066}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6109,7 +6109,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>1418</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>424</v>
       </c>
@@ -6407,7 +6407,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>425</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>514</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>519</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>520</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>525</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="9" t="s">
         <v>587</v>
       </c>
@@ -7821,7 +7821,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="9" t="s">
         <v>589</v>
       </c>
@@ -7835,7 +7835,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="9" t="s">
         <v>590</v>
       </c>
@@ -8507,7 +8507,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216" s="9" t="s">
         <v>634</v>
       </c>
@@ -8575,7 +8575,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220" s="9" t="s">
         <v>637</v>
       </c>
@@ -9991,7 +9991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="313" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A313" s="9" t="s">
         <v>693</v>
       </c>
@@ -10005,7 +10005,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="314" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A314" s="9" t="s">
         <v>694</v>
       </c>
@@ -11121,7 +11121,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="385" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A385" s="9" t="s">
         <v>753</v>
       </c>
@@ -11733,7 +11733,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="426" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A426" s="9" t="s">
         <v>781</v>
       </c>
@@ -11747,7 +11747,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="427" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A427" s="9" t="s">
         <v>782</v>
       </c>
@@ -15313,7 +15313,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="653" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A653" s="9" t="s">
         <v>973</v>
       </c>
@@ -15329,7 +15329,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="654" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="654" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A654" s="9" t="s">
         <v>974</v>
       </c>
@@ -15345,7 +15345,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="655" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="655" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A655" s="9" t="s">
         <v>975</v>
       </c>
@@ -15361,7 +15361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="656" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="656" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A656" s="9" t="s">
         <v>976</v>
       </c>
@@ -15393,7 +15393,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="658" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A658" s="9" t="s">
         <v>978</v>
       </c>
@@ -15409,7 +15409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="659" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A659" s="9" t="s">
         <v>979</v>
       </c>
@@ -15425,7 +15425,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="660" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A660" s="9" t="s">
         <v>980</v>
       </c>
@@ -15457,7 +15457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="662" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A662" s="9" t="s">
         <v>982</v>
       </c>
@@ -15473,7 +15473,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="663" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A663" s="9" t="s">
         <v>983</v>
       </c>
@@ -15489,7 +15489,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="664" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A664" s="9" t="s">
         <v>984</v>
       </c>
@@ -15521,7 +15521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="666" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A666" s="9" t="s">
         <v>986</v>
       </c>
@@ -15537,7 +15537,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="667" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A667" s="9" t="s">
         <v>987</v>
       </c>
@@ -15553,7 +15553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="668" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A668" s="9" t="s">
         <v>988</v>
       </c>
@@ -15569,7 +15569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="669" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A669" s="9" t="s">
         <v>989</v>
       </c>
@@ -15601,7 +15601,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="671" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A671" s="9" t="s">
         <v>1438</v>
       </c>
@@ -15617,7 +15617,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="672" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A672" s="9" t="s">
         <v>991</v>
       </c>
@@ -15649,7 +15649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="674" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="674" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A674" s="9" t="s">
         <v>993</v>
       </c>
@@ -15665,7 +15665,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="675" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A675" s="9" t="s">
         <v>994</v>
       </c>
@@ -15699,7 +15699,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="677" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A677" s="9" t="s">
         <v>996</v>
       </c>
@@ -15715,7 +15715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="678" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A678" s="9" t="s">
         <v>997</v>
       </c>
@@ -15731,7 +15731,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="679" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A679" s="9" t="s">
         <v>998</v>
       </c>
@@ -15827,7 +15827,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="685" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="685" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A685" s="9" t="s">
         <v>1003</v>
       </c>
@@ -15843,7 +15843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="686" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A686" s="9" t="s">
         <v>1004</v>
       </c>
@@ -15859,7 +15859,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="687" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="687" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A687" s="9" t="s">
         <v>1005</v>
       </c>
@@ -15875,7 +15875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="688" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="688" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A688" s="9" t="s">
         <v>1006</v>
       </c>
@@ -15891,7 +15891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="689" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="689" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A689" s="9" t="s">
         <v>1007</v>
       </c>
@@ -15907,7 +15907,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="690" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A690" s="9" t="s">
         <v>1008</v>
       </c>
@@ -15923,7 +15923,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="691" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="691" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A691" s="9" t="s">
         <v>1009</v>
       </c>
@@ -16023,7 +16023,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="698" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="698" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A698" s="9" t="s">
         <v>1440</v>
       </c>
@@ -16039,7 +16039,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="699" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="699" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A699" s="9" t="s">
         <v>1016</v>
       </c>
@@ -16523,7 +16523,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="731" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="731" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A731" s="9" t="s">
         <v>1045</v>
       </c>
@@ -16551,7 +16551,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="733" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="733" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A733" s="9" t="s">
         <v>1047</v>
       </c>
@@ -17128,7 +17128,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="775" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="775" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A775" s="9" t="s">
         <v>1065</v>
       </c>
@@ -17142,7 +17142,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="776" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A776" s="9" t="s">
         <v>1066</v>
       </c>
@@ -17156,7 +17156,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="777" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="777" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A777" s="9" t="s">
         <v>1067</v>
       </c>
@@ -17170,7 +17170,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="778" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="778" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A778" s="9" t="s">
         <v>1068</v>
       </c>
@@ -17386,7 +17386,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="792" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="792" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A792" s="9" t="s">
         <v>1078</v>
       </c>
@@ -19346,7 +19346,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="914" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A914" s="9" t="s">
         <v>1180</v>
       </c>
@@ -19360,7 +19360,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="915" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A915" s="9" t="s">
         <v>1181</v>
       </c>
@@ -19374,7 +19374,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="916" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A916" s="9" t="s">
         <v>1182</v>
       </c>
@@ -19388,7 +19388,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="917" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A917" s="9" t="s">
         <v>1183</v>
       </c>
@@ -19432,7 +19432,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="920" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="920" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A920" s="9" t="s">
         <v>1186</v>
       </c>
@@ -19532,7 +19532,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="926" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="926" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A926" s="9" t="s">
         <v>1192</v>
       </c>
@@ -19546,7 +19546,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="927" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A927" s="9" t="s">
         <v>1193</v>
       </c>
@@ -19560,7 +19560,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="928" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="928" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A928" s="9" t="s">
         <v>1194</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="929" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="929" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A929" s="9" t="s">
         <v>1195</v>
       </c>
@@ -19602,7 +19602,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="931" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="931" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A931" s="9" t="s">
         <v>1197</v>
       </c>
@@ -20452,7 +20452,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="983" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="983" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A983" s="9" t="s">
         <v>1243</v>
       </c>
@@ -23741,6 +23741,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F1199" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
     <filterColumn colId="4">
       <filters>
         <filter val="Core"/>
@@ -23749,6 +23752,7 @@
     </filterColumn>
     <filterColumn colId="5">
       <filters>
+        <filter val="Conversion"/>
         <filter val="FixedMemory"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Use new string resources
</commit_message>
<xml_diff>
--- a/Runtime/RuntimeFunctionsAndClasses.xlsx
+++ b/Runtime/RuntimeFunctionsAndClasses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XSharp\DevRt\Runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1B3B8227-5309-41F2-BEF3-D475FB3139A4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E063F79D-6A20-4CD6-93E3-9075CA8B00FB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6324" uniqueCount="1617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6328" uniqueCount="1617">
   <si>
     <t>function DbInfo(iInfo as INT) as OBJECT</t>
   </si>
@@ -5304,7 +5304,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E120" sqref="E120"/>
+      <selection pane="bottomLeft" activeCell="A269" sqref="A269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6612,7 +6612,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>515</v>
       </c>
@@ -7078,11 +7078,13 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>541</v>
       </c>
-      <c r="B120" s="10"/>
+      <c r="B120" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="C120" s="10"/>
       <c r="D120" s="9"/>
       <c r="E120" s="9" t="s">
@@ -7092,11 +7094,13 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>542</v>
       </c>
-      <c r="B121" s="10"/>
+      <c r="B121" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="C121" s="10"/>
       <c r="D121" s="9"/>
       <c r="E121" s="9" t="s">
@@ -10380,11 +10384,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="331" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="B331" s="10"/>
+      <c r="B331" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="C331" s="12"/>
       <c r="D331" s="9"/>
       <c r="E331" s="9" t="s">
@@ -11048,11 +11054,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="9" t="s">
         <v>740</v>
       </c>
-      <c r="B373" s="10"/>
+      <c r="B373" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="C373" s="12"/>
       <c r="D373" s="9"/>
       <c r="E373" s="9" t="s">

</xml_diff>

<commit_message>
- Added documentation comments - Created special documentation configuration with the /noclipcall commandline option for XSharp.VO
</commit_message>
<xml_diff>
--- a/Runtime/RuntimeFunctionsAndClasses.xlsx
+++ b/Runtime/RuntimeFunctionsAndClasses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XSharp\DevRt\Runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E7B695A-6217-44A1-9C41-35D74356DE79}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{44E1229D-2DCD-451A-9003-CC6E53D29D02}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5306,7 +5306,7 @@
   <dimension ref="A1:F1230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
@@ -6605,7 +6605,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>514</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>515</v>
       </c>
@@ -6637,7 +6637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>516</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>517</v>
       </c>
@@ -7457,7 +7457,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
         <v>1044</v>
       </c>
@@ -8543,7 +8543,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A208" s="9" t="s">
         <v>621</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="9" t="s">
         <v>622</v>
       </c>
@@ -8985,7 +8985,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="9" t="s">
         <v>638</v>
       </c>
@@ -9123,7 +9123,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="244" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="9" t="s">
         <v>1519</v>
       </c>
@@ -9529,7 +9529,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="268" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A268" s="9" t="s">
         <v>668</v>
       </c>
@@ -9543,7 +9543,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="269" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A269" s="9" t="s">
         <v>669</v>
       </c>
@@ -10095,7 +10095,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="306" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="9" t="s">
         <v>681</v>
       </c>
@@ -10441,7 +10441,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="327" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A327" s="9" t="s">
         <v>692</v>
       </c>
@@ -10959,7 +10959,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="359" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="9" t="s">
         <v>722</v>
       </c>
@@ -10991,7 +10991,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="361" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="9" t="s">
         <v>724</v>
       </c>
@@ -11361,7 +11361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="384" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="9" t="s">
         <v>745</v>
       </c>
@@ -11395,7 +11395,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="386" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="9" t="s">
         <v>1528</v>
       </c>
@@ -11493,7 +11493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="392" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="9" t="s">
         <v>749</v>
       </c>
@@ -11579,7 +11579,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="397" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="9" t="s">
         <v>1522</v>
       </c>
@@ -11631,7 +11631,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="400" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="9" t="s">
         <v>1531</v>
       </c>
@@ -11665,7 +11665,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="402" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="9" t="s">
         <v>1532</v>
       </c>
@@ -11681,7 +11681,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="403" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="9" t="s">
         <v>752</v>
       </c>
@@ -11697,7 +11697,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="404" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="9" t="s">
         <v>1533</v>
       </c>
@@ -12087,7 +12087,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="430" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="9" t="s">
         <v>778</v>
       </c>
@@ -12103,7 +12103,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="431" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" s="9" t="s">
         <v>1534</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="434" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" s="9" t="s">
         <v>781</v>
       </c>
@@ -12171,7 +12171,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="435" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" s="9" t="s">
         <v>1535</v>
       </c>
@@ -12203,7 +12203,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="437" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" s="9" t="s">
         <v>783</v>
       </c>
@@ -12219,7 +12219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="438" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="9" t="s">
         <v>1536</v>
       </c>
@@ -12235,7 +12235,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="439" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="9" t="s">
         <v>1537</v>
       </c>
@@ -12251,7 +12251,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="440" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="9" t="s">
         <v>784</v>
       </c>
@@ -12285,7 +12285,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="442" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" s="9" t="s">
         <v>1539</v>
       </c>
@@ -12301,7 +12301,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="443" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" s="9" t="s">
         <v>785</v>
       </c>
@@ -12385,7 +12385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="448" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" s="9" t="s">
         <v>787</v>
       </c>
@@ -12401,7 +12401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="449" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" s="9" t="s">
         <v>1541</v>
       </c>
@@ -12539,7 +12539,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="457" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" s="9" t="s">
         <v>793</v>
       </c>
@@ -12555,7 +12555,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="458" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" s="9" t="s">
         <v>1542</v>
       </c>
@@ -12571,7 +12571,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="459" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" s="9" t="s">
         <v>1543</v>
       </c>
@@ -12587,7 +12587,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="460" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" s="9" t="s">
         <v>794</v>
       </c>
@@ -12657,7 +12657,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="464" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" s="9" t="s">
         <v>795</v>
       </c>
@@ -12673,7 +12673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="465" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" s="9" t="s">
         <v>1545</v>
       </c>
@@ -12757,7 +12757,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="470" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A470" s="9" t="s">
         <v>799</v>
       </c>
@@ -12923,7 +12923,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="480" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A480" s="9" t="s">
         <v>809</v>
       </c>
@@ -12937,7 +12937,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="481" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481" s="9" t="s">
         <v>810</v>
       </c>
@@ -13003,7 +13003,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="485" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A485" s="9" t="s">
         <v>814</v>
       </c>
@@ -13017,7 +13017,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="486" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" s="9" t="s">
         <v>815</v>
       </c>
@@ -13067,7 +13067,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="489" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" s="9" t="s">
         <v>818</v>
       </c>
@@ -13083,7 +13083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="490" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" s="9" t="s">
         <v>819</v>
       </c>
@@ -13301,7 +13301,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="504" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504" s="9" t="s">
         <v>829</v>
       </c>
@@ -13317,7 +13317,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="505" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A505" s="9" t="s">
         <v>830</v>
       </c>
@@ -13403,7 +13403,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="510" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" s="9" t="s">
         <v>834</v>
       </c>
@@ -13437,7 +13437,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="512" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A512" s="9" t="s">
         <v>835</v>
       </c>
@@ -13471,7 +13471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="514" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514" s="9" t="s">
         <v>836</v>
       </c>
@@ -13539,7 +13539,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="518" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A518" s="9" t="s">
         <v>839</v>
       </c>
@@ -13673,7 +13673,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="526" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A526" s="9" t="s">
         <v>844</v>
       </c>
@@ -13807,7 +13807,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="534" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A534" s="9" t="s">
         <v>851</v>
       </c>
@@ -14021,7 +14021,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="547" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A547" s="9" t="s">
         <v>1518</v>
       </c>
@@ -14037,7 +14037,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="548" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A548" s="9" t="s">
         <v>864</v>
       </c>
@@ -14103,7 +14103,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="552" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A552" s="9" t="s">
         <v>867</v>
       </c>
@@ -14169,7 +14169,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="556" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A556" s="9" t="s">
         <v>870</v>
       </c>
@@ -15043,7 +15043,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="609" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A609" s="9" t="s">
         <v>922</v>
       </c>
@@ -16145,7 +16145,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="677" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A677" s="9" t="s">
         <v>1423</v>
       </c>
@@ -16195,7 +16195,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="680" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A680" s="9" t="s">
         <v>991</v>
       </c>
@@ -16525,7 +16525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="701" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="701" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A701" s="9" t="s">
         <v>1011</v>
       </c>
@@ -16559,7 +16559,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="703" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="703" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A703" s="9" t="s">
         <v>1425</v>
       </c>
@@ -16575,7 +16575,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="704" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="704" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A704" s="9" t="s">
         <v>1013</v>
       </c>
@@ -16591,7 +16591,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="705" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="705" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A705" s="9" t="s">
         <v>1014</v>
       </c>
@@ -16607,7 +16607,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="706" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="706" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A706" s="9" t="s">
         <v>1426</v>
       </c>
@@ -16623,7 +16623,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="707" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="707" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A707" s="9" t="s">
         <v>1015</v>
       </c>
@@ -16675,7 +16675,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="710" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="710" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A710" s="9" t="s">
         <v>1017</v>
       </c>
@@ -16981,7 +16981,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="729" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="729" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A729" s="9" t="s">
         <v>1035</v>
       </c>
@@ -17135,7 +17135,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="738" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="738" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A738" s="9" t="s">
         <v>1044</v>
       </c>
@@ -17670,7 +17670,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="776" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A776" s="9" t="s">
         <v>1058</v>
       </c>
@@ -17684,7 +17684,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="777" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="777" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A777" s="9" t="s">
         <v>1059</v>
       </c>
@@ -17898,7 +17898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="790" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="790" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A790" s="9" t="s">
         <v>1068</v>
       </c>
@@ -17914,7 +17914,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="791" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="791" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A791" s="9" t="s">
         <v>1069</v>
       </c>
@@ -17930,7 +17930,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="792" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="792" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A792" s="9" t="s">
         <v>1070</v>
       </c>
@@ -17946,7 +17946,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="793" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="793" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A793" s="9" t="s">
         <v>1071</v>
       </c>
@@ -18028,7 +18028,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="798" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="798" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A798" s="9" t="s">
         <v>1075</v>
       </c>
@@ -18364,7 +18364,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="818" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="818" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A818" s="9" t="s">
         <v>1093</v>
       </c>
@@ -18722,7 +18722,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="839" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="839" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A839" s="9" t="s">
         <v>1107</v>
       </c>
@@ -19630,7 +19630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="895" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="895" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A895" s="9" t="s">
         <v>1153</v>
       </c>
@@ -19644,7 +19644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="896" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="896" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A896" s="9" t="s">
         <v>1154</v>
       </c>
@@ -19706,7 +19706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="900" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="900" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A900" s="9" t="s">
         <v>1157</v>
       </c>
@@ -19738,7 +19738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="902" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A902" s="9" t="s">
         <v>1159</v>
       </c>
@@ -19938,7 +19938,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="914" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A914" s="9" t="s">
         <v>1171</v>
       </c>
@@ -20054,7 +20054,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="921" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A921" s="9" t="s">
         <v>1177</v>
       </c>
@@ -20102,7 +20102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="924" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A924" s="9" t="s">
         <v>1180</v>
       </c>
@@ -20152,7 +20152,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="927" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A927" s="9" t="s">
         <v>1183</v>
       </c>
@@ -20168,7 +20168,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="928" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="928" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A928" s="9" t="s">
         <v>1184</v>
       </c>
@@ -20660,7 +20660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="957" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="957" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A957" s="9" t="s">
         <v>1210</v>
       </c>
@@ -20692,7 +20692,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="959" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="959" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A959" s="9" t="s">
         <v>1212</v>
       </c>
@@ -20958,7 +20958,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="975" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="975" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A975" s="9" t="s">
         <v>1224</v>
       </c>
@@ -20972,7 +20972,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="976" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="976" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A976" s="9" t="s">
         <v>1225</v>
       </c>
@@ -20986,7 +20986,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="977" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="977" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A977" s="9" t="s">
         <v>1226</v>
       </c>
@@ -25152,9 +25152,7 @@
       </filters>
     </filterColumn>
     <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+      <filters blank="1"/>
     </filterColumn>
     <filterColumn colId="2">
       <filters blank="1"/>

</xml_diff>